<commit_message>
new fields on templates spreadsheets
</commit_message>
<xml_diff>
--- a/src/public/templates/occurrences.xlsx
+++ b/src/public/templates/occurrences.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>modified</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>occurrenceRemarks</t>
+  </si>
+  <si>
+    <t>occurrenceID</t>
+  </si>
+  <si>
+    <t>comments</t>
   </si>
 </sst>
 </file>
@@ -103,30 +109,30 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="4">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -138,7 +144,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -147,43 +153,43 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -193,10 +199,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AC1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F2" activeCellId="0" pane="topLeft" sqref="F2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC2" activeCellId="0" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -230,7 +236,7 @@
     <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -311,12 +317,18 @@
       </c>
       <c r="AA1" s="0" t="s">
         <v>26</v>
+      </c>
+      <c r="AB1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>